<commit_message>
GameScene 제작 ( 1 )
씬
GameScene 추가

스크립트
GameManager 추가
GameTimer 추가

그 외의 스크립트들 수정
</commit_message>
<xml_diff>
--- a/Unity Project/Assets/Resources/Data/KeySettingData.xlsx
+++ b/Unity Project/Assets/Resources/Data/KeySettingData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GItData\RRD\Unity Project\Assets\Resources\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyGitHub\RRD\Unity Project\Assets\Resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF7A2D3F-B67C-453A-A375-46A9CC88DF41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5005C76-AAA7-4A49-8672-0501ACCA8E11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Default" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Key</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -64,6 +64,14 @@
   </si>
   <si>
     <t>MoveRight</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KeyManager</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -420,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -471,6 +479,14 @@
         <v>9</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>